<commit_message>
Changes after meeting with Olex 28June
</commit_message>
<xml_diff>
--- a/VT_IE_SRV.xlsx
+++ b/VT_IE_SRV.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FE56ED4-63D7-4BF0-934D-B7BA17E8F186}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F3D5D78-E016-419F-9E39-29CF8D246F95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="83" r:id="rId1"/>
@@ -4416,7 +4416,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="619">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1384" uniqueCount="618">
   <si>
     <t>Unit</t>
   </si>
@@ -6425,10 +6425,7 @@
     <t>HETD</t>
   </si>
   <si>
-    <t>FT-SRVHET</t>
-  </si>
-  <si>
-    <t>CITY_DH,URBAN_1_DH,URBAN_2_DH,URBAN_3_DH</t>
+    <t>SRVHET</t>
   </si>
 </sst>
 </file>
@@ -19528,7 +19525,7 @@
     </row>
     <row r="6" spans="2:8">
       <c r="B6" s="706" t="str">
-        <f>Commodities!D38</f>
+        <f>Commodities!D41</f>
         <v>SRVCO2N</v>
       </c>
       <c r="C6" s="709">
@@ -19553,13 +19550,13 @@
     </row>
     <row r="7" spans="2:8">
       <c r="B7" s="21" t="str">
-        <f>Commodities!D39</f>
+        <f>Commodities!D42</f>
         <v>SRVCH4N</v>
       </c>
     </row>
     <row r="8" spans="2:8">
       <c r="B8" s="21" t="str">
-        <f>Commodities!D40</f>
+        <f>Commodities!D43</f>
         <v>SRVSO2N</v>
       </c>
       <c r="C8" s="25"/>
@@ -19571,7 +19568,7 @@
     </row>
     <row r="9" spans="2:8">
       <c r="B9" s="21" t="str">
-        <f>Commodities!D41</f>
+        <f>Commodities!D44</f>
         <v>SRVNOXN</v>
       </c>
       <c r="C9" s="25"/>
@@ -19583,7 +19580,7 @@
     </row>
     <row r="10" spans="2:8">
       <c r="B10" s="21" t="str">
-        <f>Commodities!D42</f>
+        <f>Commodities!D45</f>
         <v>SRVPM10</v>
       </c>
       <c r="C10" s="25"/>
@@ -19595,7 +19592,7 @@
     </row>
     <row r="11" spans="2:8">
       <c r="B11" s="31" t="str">
-        <f>Commodities!D43</f>
+        <f>Commodities!D46</f>
         <v>SRVPM25</v>
       </c>
       <c r="C11" s="126"/>
@@ -38504,17 +38501,17 @@
   <sheetPr codeName="Sheet5">
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:R98"/>
+  <dimension ref="A1:R101"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A44" sqref="A44:XFD44"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" style="30" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" style="30" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14" style="30" customWidth="1"/>
     <col min="4" max="4" width="24.28515625" style="30" customWidth="1"/>
     <col min="5" max="5" width="45" style="30" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.42578125" style="30" bestFit="1" customWidth="1"/>
@@ -39311,16 +39308,16 @@
         <v>21</v>
       </c>
       <c r="C33" s="25" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
-        <v>IE,National</v>
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:'Regions'!$AD$3)</f>
+        <v>IE,National,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
       </c>
       <c r="D33" s="30" t="str">
-        <f>Legend!C46</f>
-        <v>SRVHET</v>
+        <f>Legend!C46&amp;"_C"</f>
+        <v>SRVHET_C</v>
       </c>
       <c r="E33" s="30" t="str">
-        <f>Legend!A46&amp;" (SRV)"</f>
-        <v>District heating (SRV)</v>
+        <f>Legend!A46&amp;" (SRV) City"</f>
+        <v>District heating (SRV) City</v>
       </c>
       <c r="F33" s="30" t="s">
         <v>46</v>
@@ -39335,145 +39332,161 @@
       <c r="J33" s="30"/>
       <c r="K33" s="30"/>
     </row>
-    <row r="34" spans="1:15" s="1" customFormat="1">
-      <c r="B34" s="21" t="s">
+    <row r="34" spans="1:15" s="411" customFormat="1">
+      <c r="B34" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C34" s="21" t="str">
+      <c r="C34" s="25" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:'Regions'!$AD$3)</f>
+        <v>IE,National,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
+      </c>
+      <c r="D34" s="30" t="str">
+        <f>Legend!C46&amp;"_1"</f>
+        <v>SRVHET_1</v>
+      </c>
+      <c r="E34" s="30" t="str">
+        <f>Legend!A46&amp;" (SRV) High Density Urban"</f>
+        <v>District heating (SRV) High Density Urban</v>
+      </c>
+      <c r="F34" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G34" s="30" t="s">
+        <v>154</v>
+      </c>
+      <c r="H34" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="I34" s="30"/>
+      <c r="J34" s="30"/>
+      <c r="K34" s="30"/>
+    </row>
+    <row r="35" spans="1:15" s="411" customFormat="1">
+      <c r="B35" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C35" s="25" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:'Regions'!$AD$3)</f>
+        <v>IE,National,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
+      </c>
+      <c r="D35" s="30" t="str">
+        <f>Legend!C46&amp;"_2"</f>
+        <v>SRVHET_2</v>
+      </c>
+      <c r="E35" s="30" t="str">
+        <f>Legend!A46&amp;" (SRV) Medium Density Urban"</f>
+        <v>District heating (SRV) Medium Density Urban</v>
+      </c>
+      <c r="F35" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G35" s="30" t="s">
+        <v>154</v>
+      </c>
+      <c r="H35" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="I35" s="30"/>
+      <c r="J35" s="30"/>
+      <c r="K35" s="30"/>
+    </row>
+    <row r="36" spans="1:15" s="411" customFormat="1">
+      <c r="B36" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C36" s="25" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:'Regions'!$AD$3)</f>
+        <v>IE,National,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
+      </c>
+      <c r="D36" s="30" t="str">
+        <f>Legend!C46&amp;"_3"</f>
+        <v>SRVHET_3</v>
+      </c>
+      <c r="E36" s="30" t="str">
+        <f>Legend!A46&amp;" (SRV) Low Density Urban"</f>
+        <v>District heating (SRV) Low Density Urban</v>
+      </c>
+      <c r="F36" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="G36" s="30" t="s">
+        <v>154</v>
+      </c>
+      <c r="H36" s="30" t="s">
+        <v>88</v>
+      </c>
+      <c r="I36" s="30"/>
+      <c r="J36" s="30"/>
+      <c r="K36" s="30"/>
+    </row>
+    <row r="37" spans="1:15" s="1" customFormat="1">
+      <c r="B37" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C37" s="21" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
         <v>IE,National</v>
       </c>
-      <c r="D34" s="21" t="str">
+      <c r="D37" s="21" t="str">
         <f>Legend!C47</f>
         <v>SRVWIN</v>
       </c>
-      <c r="E34" s="21" t="str">
+      <c r="E37" s="21" t="str">
         <f>Legend!A47&amp;" (SRV)"</f>
         <v>Wind (SRV)</v>
       </c>
-      <c r="F34" s="21" t="s">
+      <c r="F37" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="G34" s="102"/>
-      <c r="H34" s="102"/>
-      <c r="I34" s="102"/>
-      <c r="J34" s="102"/>
-      <c r="K34" s="30"/>
-    </row>
-    <row r="35" spans="1:15" s="1" customFormat="1">
-      <c r="B35" s="21" t="s">
+      <c r="G37" s="102"/>
+      <c r="H37" s="102"/>
+      <c r="I37" s="102"/>
+      <c r="J37" s="102"/>
+      <c r="K37" s="30"/>
+    </row>
+    <row r="38" spans="1:15" s="1" customFormat="1">
+      <c r="B38" s="21" t="s">
         <v>21</v>
-      </c>
-      <c r="C35" s="21" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
-        <v>IE,National</v>
-      </c>
-      <c r="D35" s="21" t="str">
-        <f>Legend!C48</f>
-        <v>SRVH2G</v>
-      </c>
-      <c r="E35" s="21" t="str">
-        <f>Legend!A48&amp;" (SRV)"</f>
-        <v>Hydrogen (gaseous) (SRV)</v>
-      </c>
-      <c r="F35" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="G35" s="21"/>
-      <c r="H35" s="21"/>
-      <c r="I35" s="21"/>
-      <c r="J35" s="21"/>
-      <c r="K35" s="30"/>
-    </row>
-    <row r="36" spans="1:15" s="1" customFormat="1">
-      <c r="B36" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="C36" s="21" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
-        <v>IE,National</v>
-      </c>
-      <c r="D36" s="21" t="str">
-        <f>Legend!C49</f>
-        <v>SRVH2L</v>
-      </c>
-      <c r="E36" s="21" t="str">
-        <f>Legend!A49&amp;" (SRV)"</f>
-        <v>Hydrogen (liquid) (SRV)</v>
-      </c>
-      <c r="F36" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="G36" s="102"/>
-      <c r="H36" s="102"/>
-      <c r="I36" s="102"/>
-      <c r="J36" s="102"/>
-      <c r="K36" s="30"/>
-    </row>
-    <row r="37" spans="1:15" s="1" customFormat="1">
-      <c r="B37" s="31" t="s">
-        <v>21</v>
-      </c>
-      <c r="C37" s="31" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
-        <v>IE,National</v>
-      </c>
-      <c r="D37" s="31" t="str">
-        <f>Legend!C50</f>
-        <v>SRVBDL</v>
-      </c>
-      <c r="E37" s="31" t="str">
-        <f>Legend!A50&amp;" (SRV)"</f>
-        <v>Biodiesel (SRV)</v>
-      </c>
-      <c r="F37" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="G37" s="103"/>
-      <c r="H37" s="103"/>
-      <c r="I37" s="103"/>
-      <c r="J37" s="103"/>
-      <c r="K37" s="30"/>
-    </row>
-    <row r="38" spans="1:15" s="1" customFormat="1">
-      <c r="B38" s="663" t="s">
-        <v>26</v>
       </c>
       <c r="C38" s="21" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
         <v>IE,National</v>
       </c>
-      <c r="D38" s="17" t="s">
-        <v>531</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>542</v>
-      </c>
-      <c r="F38" s="663" t="s">
-        <v>543</v>
-      </c>
-      <c r="G38" s="663"/>
-      <c r="H38" s="663"/>
-      <c r="I38" s="663"/>
-      <c r="J38" s="663"/>
+      <c r="D38" s="21" t="str">
+        <f>Legend!C48</f>
+        <v>SRVH2G</v>
+      </c>
+      <c r="E38" s="21" t="str">
+        <f>Legend!A48&amp;" (SRV)"</f>
+        <v>Hydrogen (gaseous) (SRV)</v>
+      </c>
+      <c r="F38" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="21"/>
       <c r="K38" s="30"/>
     </row>
     <row r="39" spans="1:15" s="1" customFormat="1">
       <c r="B39" s="21" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C39" s="21" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
         <v>IE,National</v>
       </c>
-      <c r="D39" s="454" t="s">
-        <v>532</v>
-      </c>
-      <c r="E39" s="102" t="s">
-        <v>537</v>
-      </c>
-      <c r="F39" s="102" t="s">
-        <v>543</v>
+      <c r="D39" s="21" t="str">
+        <f>Legend!C49</f>
+        <v>SRVH2L</v>
+      </c>
+      <c r="E39" s="21" t="str">
+        <f>Legend!A49&amp;" (SRV)"</f>
+        <v>Hydrogen (liquid) (SRV)</v>
+      </c>
+      <c r="F39" s="21" t="s">
+        <v>46</v>
       </c>
       <c r="G39" s="102"/>
       <c r="H39" s="102"/>
@@ -39482,49 +39495,51 @@
       <c r="K39" s="30"/>
     </row>
     <row r="40" spans="1:15" s="1" customFormat="1">
-      <c r="B40" s="21" t="s">
-        <v>26</v>
-      </c>
-      <c r="C40" s="21" t="str">
+      <c r="B40" s="31" t="s">
+        <v>21</v>
+      </c>
+      <c r="C40" s="31" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
         <v>IE,National</v>
       </c>
-      <c r="D40" s="12" t="s">
-        <v>533</v>
-      </c>
-      <c r="E40" s="102" t="s">
-        <v>538</v>
-      </c>
-      <c r="F40" s="102" t="s">
-        <v>543</v>
-      </c>
-      <c r="G40" s="21"/>
-      <c r="H40" s="21"/>
-      <c r="I40" s="21"/>
-      <c r="J40" s="21"/>
+      <c r="D40" s="31" t="str">
+        <f>Legend!C50</f>
+        <v>SRVBDL</v>
+      </c>
+      <c r="E40" s="31" t="str">
+        <f>Legend!A50&amp;" (SRV)"</f>
+        <v>Biodiesel (SRV)</v>
+      </c>
+      <c r="F40" s="31" t="s">
+        <v>46</v>
+      </c>
+      <c r="G40" s="103"/>
+      <c r="H40" s="103"/>
+      <c r="I40" s="103"/>
+      <c r="J40" s="103"/>
       <c r="K40" s="30"/>
     </row>
     <row r="41" spans="1:15" s="1" customFormat="1">
-      <c r="B41" s="21" t="s">
+      <c r="B41" s="663" t="s">
         <v>26</v>
       </c>
       <c r="C41" s="21" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
         <v>IE,National</v>
       </c>
-      <c r="D41" s="12" t="s">
-        <v>534</v>
-      </c>
-      <c r="E41" s="102" t="s">
-        <v>539</v>
-      </c>
-      <c r="F41" s="102" t="s">
+      <c r="D41" s="17" t="s">
+        <v>531</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>542</v>
+      </c>
+      <c r="F41" s="663" t="s">
         <v>543</v>
       </c>
-      <c r="G41" s="21"/>
-      <c r="H41" s="21"/>
-      <c r="I41" s="21"/>
-      <c r="J41" s="21"/>
+      <c r="G41" s="663"/>
+      <c r="H41" s="663"/>
+      <c r="I41" s="663"/>
+      <c r="J41" s="663"/>
       <c r="K41" s="30"/>
     </row>
     <row r="42" spans="1:15" s="1" customFormat="1">
@@ -39535,166 +39550,217 @@
         <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
         <v>IE,National</v>
       </c>
-      <c r="D42" s="12" t="s">
-        <v>535</v>
+      <c r="D42" s="454" t="s">
+        <v>532</v>
       </c>
       <c r="E42" s="102" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="F42" s="102" t="s">
         <v>543</v>
       </c>
-      <c r="G42" s="21"/>
-      <c r="H42" s="21"/>
-      <c r="I42" s="21"/>
-      <c r="J42" s="21"/>
+      <c r="G42" s="102"/>
+      <c r="H42" s="102"/>
+      <c r="I42" s="102"/>
+      <c r="J42" s="102"/>
       <c r="K42" s="30"/>
     </row>
     <row r="43" spans="1:15" s="1" customFormat="1">
-      <c r="B43" s="31" t="s">
+      <c r="B43" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="C43" s="31" t="str">
+      <c r="C43" s="21" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
         <v>IE,National</v>
       </c>
-      <c r="D43" s="14" t="s">
+      <c r="D43" s="12" t="s">
+        <v>533</v>
+      </c>
+      <c r="E43" s="102" t="s">
+        <v>538</v>
+      </c>
+      <c r="F43" s="102" t="s">
+        <v>543</v>
+      </c>
+      <c r="G43" s="21"/>
+      <c r="H43" s="21"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="21"/>
+      <c r="K43" s="30"/>
+    </row>
+    <row r="44" spans="1:15" s="1" customFormat="1">
+      <c r="B44" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C44" s="21" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
+        <v>IE,National</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>534</v>
+      </c>
+      <c r="E44" s="102" t="s">
+        <v>539</v>
+      </c>
+      <c r="F44" s="102" t="s">
+        <v>543</v>
+      </c>
+      <c r="G44" s="21"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="21"/>
+      <c r="J44" s="21"/>
+      <c r="K44" s="30"/>
+    </row>
+    <row r="45" spans="1:15" s="1" customFormat="1">
+      <c r="B45" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C45" s="21" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
+        <v>IE,National</v>
+      </c>
+      <c r="D45" s="12" t="s">
+        <v>535</v>
+      </c>
+      <c r="E45" s="102" t="s">
+        <v>540</v>
+      </c>
+      <c r="F45" s="102" t="s">
+        <v>543</v>
+      </c>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
+      <c r="K45" s="30"/>
+    </row>
+    <row r="46" spans="1:15" s="1" customFormat="1">
+      <c r="B46" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="C46" s="31" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
+        <v>IE,National</v>
+      </c>
+      <c r="D46" s="14" t="s">
         <v>536</v>
       </c>
-      <c r="E43" s="103" t="s">
+      <c r="E46" s="103" t="s">
         <v>541</v>
       </c>
-      <c r="F43" s="103" t="s">
+      <c r="F46" s="103" t="s">
         <v>543</v>
       </c>
-      <c r="G43" s="31"/>
-      <c r="H43" s="31"/>
-      <c r="I43" s="31"/>
-      <c r="J43" s="31"/>
-      <c r="K43" s="30"/>
-    </row>
-    <row r="44" spans="1:15" s="1" customFormat="1">
-      <c r="B44" s="30"/>
-      <c r="C44" s="30"/>
-      <c r="D44" s="7"/>
-      <c r="G44" s="30"/>
-      <c r="H44" s="30"/>
-      <c r="I44" s="30"/>
-      <c r="J44" s="30"/>
-      <c r="K44" s="30"/>
-    </row>
-    <row r="45" spans="1:15">
-      <c r="A45" s="1"/>
-      <c r="L45" s="4"/>
-      <c r="M45" s="4"/>
-      <c r="N45" s="4"/>
-      <c r="O45" s="4"/>
-    </row>
-    <row r="46" spans="1:15">
-      <c r="A46" s="1"/>
-      <c r="L46" s="4"/>
-      <c r="M46" s="4"/>
-      <c r="N46" s="4"/>
-      <c r="O46" s="4"/>
-    </row>
-    <row r="47" spans="1:15">
-      <c r="A47" s="1"/>
-      <c r="L47" s="4"/>
-      <c r="M47" s="4"/>
-      <c r="N47" s="4"/>
-      <c r="O47" s="4"/>
+      <c r="G46" s="31"/>
+      <c r="H46" s="31"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="31"/>
+      <c r="K46" s="30"/>
+    </row>
+    <row r="47" spans="1:15" s="1" customFormat="1">
+      <c r="B47" s="30"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="7"/>
+      <c r="G47" s="30"/>
+      <c r="H47" s="30"/>
+      <c r="I47" s="30"/>
+      <c r="J47" s="30"/>
+      <c r="K47" s="30"/>
     </row>
     <row r="48" spans="1:15">
+      <c r="A48" s="1"/>
       <c r="L48" s="4"/>
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
       <c r="O48" s="4"/>
     </row>
-    <row r="49" spans="12:15">
+    <row r="49" spans="1:15">
+      <c r="A49" s="1"/>
       <c r="L49" s="4"/>
       <c r="M49" s="4"/>
       <c r="N49" s="4"/>
       <c r="O49" s="4"/>
     </row>
-    <row r="50" spans="12:15">
+    <row r="50" spans="1:15">
+      <c r="A50" s="1"/>
       <c r="L50" s="4"/>
       <c r="M50" s="4"/>
       <c r="N50" s="4"/>
       <c r="O50" s="4"/>
     </row>
-    <row r="52" spans="12:15">
+    <row r="51" spans="1:15">
+      <c r="L51" s="4"/>
+      <c r="M51" s="4"/>
+      <c r="N51" s="4"/>
+      <c r="O51" s="4"/>
+    </row>
+    <row r="52" spans="1:15">
       <c r="L52" s="4"/>
       <c r="M52" s="4"/>
       <c r="N52" s="4"/>
       <c r="O52" s="4"/>
     </row>
-    <row r="53" spans="12:15">
+    <row r="53" spans="1:15">
       <c r="L53" s="4"/>
       <c r="M53" s="4"/>
       <c r="N53" s="4"/>
       <c r="O53" s="4"/>
     </row>
-    <row r="54" spans="12:15">
-      <c r="L54" s="4"/>
-      <c r="M54" s="4"/>
-      <c r="N54" s="4"/>
-      <c r="O54" s="4"/>
-    </row>
-    <row r="55" spans="12:15">
+    <row r="55" spans="1:15">
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
       <c r="O55" s="4"/>
     </row>
-    <row r="56" spans="12:15">
+    <row r="56" spans="1:15">
       <c r="L56" s="4"/>
       <c r="M56" s="4"/>
       <c r="N56" s="4"/>
       <c r="O56" s="4"/>
     </row>
-    <row r="57" spans="12:15">
+    <row r="57" spans="1:15">
       <c r="L57" s="4"/>
       <c r="M57" s="4"/>
       <c r="N57" s="4"/>
       <c r="O57" s="4"/>
     </row>
-    <row r="58" spans="12:15">
+    <row r="58" spans="1:15">
       <c r="L58" s="4"/>
       <c r="M58" s="4"/>
       <c r="N58" s="4"/>
       <c r="O58" s="4"/>
     </row>
-    <row r="59" spans="12:15">
+    <row r="59" spans="1:15">
       <c r="L59" s="4"/>
       <c r="M59" s="4"/>
       <c r="N59" s="4"/>
       <c r="O59" s="4"/>
     </row>
-    <row r="60" spans="12:15">
+    <row r="60" spans="1:15">
       <c r="L60" s="4"/>
       <c r="M60" s="4"/>
       <c r="N60" s="4"/>
       <c r="O60" s="4"/>
     </row>
-    <row r="61" spans="12:15">
+    <row r="61" spans="1:15">
       <c r="L61" s="4"/>
       <c r="M61" s="4"/>
       <c r="N61" s="4"/>
       <c r="O61" s="4"/>
     </row>
-    <row r="62" spans="12:15">
+    <row r="62" spans="1:15">
       <c r="L62" s="4"/>
       <c r="M62" s="4"/>
       <c r="N62" s="4"/>
       <c r="O62" s="4"/>
     </row>
-    <row r="63" spans="12:15">
+    <row r="63" spans="1:15">
       <c r="L63" s="4"/>
       <c r="M63" s="4"/>
       <c r="N63" s="4"/>
       <c r="O63" s="4"/>
     </row>
-    <row r="64" spans="12:15">
+    <row r="64" spans="1:15">
       <c r="L64" s="4"/>
       <c r="M64" s="4"/>
       <c r="N64" s="4"/>
@@ -39903,6 +39969,24 @@
       <c r="M98" s="4"/>
       <c r="N98" s="4"/>
       <c r="O98" s="4"/>
+    </row>
+    <row r="99" spans="12:15">
+      <c r="L99" s="4"/>
+      <c r="M99" s="4"/>
+      <c r="N99" s="4"/>
+      <c r="O99" s="4"/>
+    </row>
+    <row r="100" spans="12:15">
+      <c r="L100" s="4"/>
+      <c r="M100" s="4"/>
+      <c r="N100" s="4"/>
+      <c r="O100" s="4"/>
+    </row>
+    <row r="101" spans="12:15">
+      <c r="L101" s="4"/>
+      <c r="M101" s="4"/>
+      <c r="N101" s="4"/>
+      <c r="O101" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -39914,10 +39998,10 @@
   <sheetPr codeName="Sheet6">
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:Q22"/>
+  <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -40426,12 +40510,13 @@
         <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:'Regions'!$AD$3)</f>
         <v>IE,National,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
       </c>
-      <c r="K14" s="63" t="s">
-        <v>617</v>
+      <c r="K14" s="63" t="str">
+        <f>"FT-"&amp;Commodities!D33</f>
+        <v>FT-SRVHET_C</v>
       </c>
       <c r="L14" s="63" t="str">
-        <f>"Fuel Tech - "&amp;Legend!A46</f>
-        <v>Fuel Tech - District heating</v>
+        <f>Commodities!E33</f>
+        <v>District heating (SRV) City</v>
       </c>
       <c r="M14" s="63" t="s">
         <v>46</v>
@@ -40465,16 +40550,16 @@
         <v>24</v>
       </c>
       <c r="J15" s="63" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
-        <v>IE,National</v>
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:'Regions'!$AD$3)</f>
+        <v>IE,National,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
       </c>
       <c r="K15" s="63" t="str">
-        <f>"FT-"&amp;D18</f>
-        <v>FT-SRVWIN</v>
+        <f>"FT-"&amp;Commodities!D34</f>
+        <v>FT-SRVHET_1</v>
       </c>
       <c r="L15" s="63" t="str">
-        <f>"Fuel Tech - "&amp;Legend!A47</f>
-        <v>Fuel Tech - Wind</v>
+        <f>Commodities!E34</f>
+        <v>District heating (SRV) High Density Urban</v>
       </c>
       <c r="M15" s="63" t="s">
         <v>46</v>
@@ -40482,7 +40567,9 @@
       <c r="N15" s="63" t="s">
         <v>592</v>
       </c>
-      <c r="O15" s="63"/>
+      <c r="O15" s="63" t="s">
+        <v>88</v>
+      </c>
       <c r="P15" s="63"/>
     </row>
     <row r="16" spans="2:17">
@@ -40499,16 +40586,16 @@
         <v>24</v>
       </c>
       <c r="J16" s="63" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
-        <v>IE,National</v>
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:'Regions'!$AD$3)</f>
+        <v>IE,National,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
       </c>
       <c r="K16" s="63" t="str">
-        <f>"FT-"&amp;D19</f>
-        <v>FT-SRVH2G</v>
+        <f>"FT-"&amp;Commodities!D35</f>
+        <v>FT-SRVHET_2</v>
       </c>
       <c r="L16" s="63" t="str">
-        <f>"Fuel Tech - "&amp;Legend!A48</f>
-        <v>Fuel Tech - Hydrogen (gaseous)</v>
+        <f>Commodities!E35</f>
+        <v>District heating (SRV) Medium Density Urban</v>
       </c>
       <c r="M16" s="63" t="s">
         <v>46</v>
@@ -40516,19 +40603,21 @@
       <c r="N16" s="63" t="s">
         <v>592</v>
       </c>
-      <c r="O16" s="63"/>
+      <c r="O16" s="63" t="s">
+        <v>88</v>
+      </c>
       <c r="P16" s="63"/>
     </row>
     <row r="17" spans="2:17">
       <c r="B17" s="729" t="str">
-        <f>K14</f>
-        <v>FT-SRVHET</v>
+        <f t="shared" ref="B17:B20" si="4">K14</f>
+        <v>FT-SRVHET_C</v>
       </c>
       <c r="C17" s="728" t="s">
         <v>616</v>
       </c>
       <c r="D17" s="663" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="E17" s="663">
         <v>1</v>
@@ -40539,16 +40628,16 @@
         <v>24</v>
       </c>
       <c r="J17" s="63" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
-        <v>IE,National</v>
+        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:'Regions'!$AD$3)</f>
+        <v>IE,National,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
       </c>
       <c r="K17" s="63" t="str">
-        <f>"FT-"&amp;D20</f>
-        <v>FT-SRVH2L</v>
+        <f>"FT-"&amp;Commodities!D36</f>
+        <v>FT-SRVHET_3</v>
       </c>
       <c r="L17" s="63" t="str">
-        <f>"Fuel Tech - "&amp;Legend!A49</f>
-        <v>Fuel Tech - Hydrogen (liquid)</v>
+        <f>Commodities!E36</f>
+        <v>District heating (SRV) Low Density Urban</v>
       </c>
       <c r="M17" s="63" t="s">
         <v>46</v>
@@ -40556,24 +40645,27 @@
       <c r="N17" s="63" t="s">
         <v>592</v>
       </c>
-      <c r="O17" s="63"/>
+      <c r="O17" s="63" t="s">
+        <v>88</v>
+      </c>
       <c r="P17" s="63"/>
     </row>
     <row r="18" spans="2:17">
-      <c r="B18" s="30" t="str">
-        <f>K15</f>
-        <v>FT-SRVWIN</v>
-      </c>
-      <c r="C18" s="30" t="s">
-        <v>564</v>
-      </c>
-      <c r="D18" s="30" t="str">
-        <f>Legend!C47</f>
-        <v>SRVWIN</v>
-      </c>
-      <c r="E18" s="30">
+      <c r="B18" s="729" t="str">
+        <f t="shared" si="4"/>
+        <v>FT-SRVHET_1</v>
+      </c>
+      <c r="C18" s="728" t="s">
+        <v>616</v>
+      </c>
+      <c r="D18" s="663" t="s">
+        <v>617</v>
+      </c>
+      <c r="E18" s="663">
         <v>1</v>
       </c>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
       <c r="I18" s="63" t="s">
         <v>24</v>
       </c>
@@ -40583,11 +40675,11 @@
       </c>
       <c r="K18" s="63" t="str">
         <f>"FT-"&amp;D21</f>
-        <v>FT-SRVBDL</v>
+        <v>FT-SRVWIN</v>
       </c>
       <c r="L18" s="63" t="str">
-        <f>"Fuel Tech - "&amp;Legend!A50</f>
-        <v>Fuel Tech - Biodiesel</v>
+        <f>"Fuel Tech - "&amp;Legend!A47</f>
+        <v>Fuel Tech - Wind</v>
       </c>
       <c r="M18" s="63" t="s">
         <v>46</v>
@@ -40599,94 +40691,213 @@
       <c r="P18" s="63"/>
     </row>
     <row r="19" spans="2:17">
-      <c r="B19" s="30" t="str">
-        <f>K16</f>
-        <v>FT-SRVH2G</v>
-      </c>
-      <c r="C19" s="30" t="s">
-        <v>565</v>
-      </c>
-      <c r="D19" s="30" t="str">
-        <f>Legend!C48</f>
-        <v>SRVH2G</v>
-      </c>
-      <c r="E19" s="30">
+      <c r="B19" s="729" t="str">
+        <f t="shared" si="4"/>
+        <v>FT-SRVHET_2</v>
+      </c>
+      <c r="C19" s="728" t="s">
+        <v>616</v>
+      </c>
+      <c r="D19" s="663" t="s">
+        <v>617</v>
+      </c>
+      <c r="E19" s="663">
         <v>1</v>
       </c>
-      <c r="I19" s="65" t="s">
+      <c r="F19" s="21"/>
+      <c r="G19" s="21"/>
+      <c r="I19" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="J19" s="65" t="str">
+      <c r="J19" s="63" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
         <v>IE,National</v>
       </c>
-      <c r="K19" s="65" t="str">
+      <c r="K19" s="63" t="str">
         <f>"FT-"&amp;D22</f>
-        <v>FT-SRVETH</v>
-      </c>
-      <c r="L19" s="65" t="str">
-        <f>"Fuel Tech - "&amp;Legend!A51</f>
-        <v>Fuel Tech - Ethanol</v>
-      </c>
-      <c r="M19" s="65" t="s">
+        <v>FT-SRVH2G</v>
+      </c>
+      <c r="L19" s="63" t="str">
+        <f>"Fuel Tech - "&amp;Legend!A48</f>
+        <v>Fuel Tech - Hydrogen (gaseous)</v>
+      </c>
+      <c r="M19" s="63" t="s">
         <v>46</v>
       </c>
-      <c r="N19" s="65" t="s">
+      <c r="N19" s="63" t="s">
         <v>592</v>
       </c>
-      <c r="O19" s="65"/>
-      <c r="P19" s="65"/>
-      <c r="Q19" s="31"/>
+      <c r="O19" s="63"/>
+      <c r="P19" s="63"/>
     </row>
     <row r="20" spans="2:17">
-      <c r="B20" s="30" t="str">
-        <f>K17</f>
+      <c r="B20" s="729" t="str">
+        <f t="shared" si="4"/>
+        <v>FT-SRVHET_3</v>
+      </c>
+      <c r="C20" s="728" t="s">
+        <v>616</v>
+      </c>
+      <c r="D20" s="663" t="s">
+        <v>617</v>
+      </c>
+      <c r="E20" s="663">
+        <v>1</v>
+      </c>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
+      <c r="I20" s="63" t="s">
+        <v>24</v>
+      </c>
+      <c r="J20" s="63" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
+        <v>IE,National</v>
+      </c>
+      <c r="K20" s="63" t="str">
+        <f>"FT-"&amp;D23</f>
         <v>FT-SRVH2L</v>
       </c>
-      <c r="C20" s="30" t="s">
-        <v>570</v>
-      </c>
-      <c r="D20" s="30" t="str">
-        <f>Legend!C49</f>
-        <v>SRVH2L</v>
-      </c>
-      <c r="E20" s="30">
-        <v>1</v>
-      </c>
+      <c r="L20" s="63" t="str">
+        <f>"Fuel Tech - "&amp;Legend!A49</f>
+        <v>Fuel Tech - Hydrogen (liquid)</v>
+      </c>
+      <c r="M20" s="63" t="s">
+        <v>46</v>
+      </c>
+      <c r="N20" s="63" t="s">
+        <v>592</v>
+      </c>
+      <c r="O20" s="63"/>
+      <c r="P20" s="63"/>
     </row>
     <row r="21" spans="2:17">
       <c r="B21" s="30" t="str">
         <f>K18</f>
+        <v>FT-SRVWIN</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>564</v>
+      </c>
+      <c r="D21" s="30" t="str">
+        <f>Legend!C47</f>
+        <v>SRVWIN</v>
+      </c>
+      <c r="E21" s="30">
+        <v>1</v>
+      </c>
+      <c r="I21" s="63" t="s">
+        <v>24</v>
+      </c>
+      <c r="J21" s="63" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
+        <v>IE,National</v>
+      </c>
+      <c r="K21" s="63" t="str">
+        <f>"FT-"&amp;D24</f>
         <v>FT-SRVBDL</v>
       </c>
-      <c r="C21" s="30" t="s">
+      <c r="L21" s="63" t="str">
+        <f>"Fuel Tech - "&amp;Legend!A50</f>
+        <v>Fuel Tech - Biodiesel</v>
+      </c>
+      <c r="M21" s="63" t="s">
+        <v>46</v>
+      </c>
+      <c r="N21" s="63" t="s">
+        <v>592</v>
+      </c>
+      <c r="O21" s="63"/>
+      <c r="P21" s="63"/>
+    </row>
+    <row r="22" spans="2:17">
+      <c r="B22" s="30" t="str">
+        <f>K19</f>
+        <v>FT-SRVH2G</v>
+      </c>
+      <c r="C22" s="30" t="s">
+        <v>565</v>
+      </c>
+      <c r="D22" s="30" t="str">
+        <f>Legend!C48</f>
+        <v>SRVH2G</v>
+      </c>
+      <c r="E22" s="30">
+        <v>1</v>
+      </c>
+      <c r="I22" s="65" t="s">
+        <v>24</v>
+      </c>
+      <c r="J22" s="65" t="str">
+        <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
+        <v>IE,National</v>
+      </c>
+      <c r="K22" s="65" t="str">
+        <f>"FT-"&amp;D25</f>
+        <v>FT-SRVETH</v>
+      </c>
+      <c r="L22" s="65" t="str">
+        <f>"Fuel Tech - "&amp;Legend!A51</f>
+        <v>Fuel Tech - Ethanol</v>
+      </c>
+      <c r="M22" s="65" t="s">
+        <v>46</v>
+      </c>
+      <c r="N22" s="65" t="s">
+        <v>592</v>
+      </c>
+      <c r="O22" s="65"/>
+      <c r="P22" s="65"/>
+      <c r="Q22" s="31"/>
+    </row>
+    <row r="23" spans="2:17">
+      <c r="B23" s="30" t="str">
+        <f>K20</f>
+        <v>FT-SRVH2L</v>
+      </c>
+      <c r="C23" s="30" t="s">
+        <v>570</v>
+      </c>
+      <c r="D23" s="30" t="str">
+        <f>Legend!C49</f>
+        <v>SRVH2L</v>
+      </c>
+      <c r="E23" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:17">
+      <c r="B24" s="30" t="str">
+        <f>K21</f>
+        <v>FT-SRVBDL</v>
+      </c>
+      <c r="C24" s="30" t="s">
         <v>561</v>
       </c>
-      <c r="D21" s="30" t="str">
+      <c r="D24" s="30" t="str">
         <f>Legend!C50</f>
         <v>SRVBDL</v>
       </c>
-      <c r="E21" s="30">
+      <c r="E24" s="30">
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:17">
-      <c r="B22" s="31" t="str">
-        <f>K19</f>
+    <row r="25" spans="2:17">
+      <c r="B25" s="31" t="str">
+        <f>K22</f>
         <v>FT-SRVETH</v>
       </c>
-      <c r="C22" s="31" t="s">
+      <c r="C25" s="31" t="s">
         <v>560</v>
       </c>
-      <c r="D22" s="31" t="str">
+      <c r="D25" s="31" t="str">
         <f>Legend!C51</f>
         <v>SRVETH</v>
       </c>
-      <c r="E22" s="31">
+      <c r="E25" s="31">
         <v>1</v>
       </c>
-      <c r="F22" s="31"/>
-      <c r="G22" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Seperate out RSDHET_C and SRVHET_C
</commit_message>
<xml_diff>
--- a/VT_IE_SRV.xlsx
+++ b/VT_IE_SRV.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A963294F-88DF-4A4B-9EF5-AAD6D386AD6D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC580AA-A9CC-485A-B52A-9C2670A6AF36}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="83" r:id="rId1"/>
@@ -30218,8 +30218,8 @@
   </sheetPr>
   <dimension ref="A1:C66"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C51" sqref="C51"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A32" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -38513,8 +38513,8 @@
   </sheetPr>
   <dimension ref="A1:R98"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33:J33"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -39326,8 +39326,8 @@
         <v>SRVHET</v>
       </c>
       <c r="E33" s="731" t="str">
-        <f>Legend!A46</f>
-        <v>District heating</v>
+        <f>Legend!A46&amp;" (SRV)"</f>
+        <v>District heating (SRV)</v>
       </c>
       <c r="F33" s="731" t="s">
         <v>46</v>
@@ -39923,8 +39923,8 @@
   </sheetPr>
   <dimension ref="A1:Q25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -40439,7 +40439,7 @@
       </c>
       <c r="L14" s="63" t="str">
         <f>Commodities!E33&amp;" in City"</f>
-        <v>District heating in City</v>
+        <v>District heating (SRV) in City</v>
       </c>
       <c r="M14" s="63" t="s">
         <v>46</v>
@@ -40482,7 +40482,7 @@
       </c>
       <c r="L15" s="63" t="str">
         <f>Commodities!E33&amp;" in High Urban Density"</f>
-        <v>District heating in High Urban Density</v>
+        <v>District heating (SRV) in High Urban Density</v>
       </c>
       <c r="M15" s="63" t="s">
         <v>46</v>
@@ -40518,7 +40518,7 @@
       </c>
       <c r="L16" s="63" t="str">
         <f>Commodities!E33&amp;" in Medium Urban Density"</f>
-        <v>District heating in Medium Urban Density</v>
+        <v>District heating (SRV) in Medium Urban Density</v>
       </c>
       <c r="M16" s="63" t="s">
         <v>46</v>
@@ -40560,7 +40560,7 @@
       </c>
       <c r="L17" s="63" t="str">
         <f>Commodities!E33&amp;" in Low Urban Density"</f>
-        <v>District heating in Low Urban Density</v>
+        <v>District heating (SRV) in Low Urban Density</v>
       </c>
       <c r="M17" s="63" t="s">
         <v>46</v>

</xml_diff>

<commit_message>
Update for new DH flow variables
</commit_message>
<xml_diff>
--- a/VT_IE_SRV.xlsx
+++ b/VT_IE_SRV.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git_TIMES Models\Irish-TIMES-model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8750B92E-3805-4309-980F-AC7BFFEDEC06}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC506381-39CC-407D-ABB5-87783E9011E8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-8145" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="83" r:id="rId1"/>
@@ -4416,7 +4416,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1371" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1353" uniqueCount="617">
   <si>
     <t>Unit</t>
   </si>
@@ -38513,7 +38513,7 @@
   </sheetPr>
   <dimension ref="A1:R98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
@@ -39919,10 +39919,10 @@
   <sheetPr codeName="Sheet6">
     <tabColor theme="9" tint="0.59999389629810485"/>
   </sheetPr>
-  <dimension ref="A1:Q25"/>
+  <dimension ref="A1:Q22"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L24" sqref="L24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -40432,12 +40432,12 @@
         <v>IE,National,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
       </c>
       <c r="K14" s="63" t="str">
-        <f>"FT-"&amp;Commodities!D33&amp;"_C"</f>
-        <v>FT-SRVHET_C</v>
+        <f>"FT-"&amp;Commodities!D33&amp;"_X"</f>
+        <v>FT-SRVHET_X</v>
       </c>
       <c r="L14" s="63" t="str">
-        <f>Commodities!E33&amp;" in City"</f>
-        <v>District heating (SRV) in City</v>
+        <f>Commodities!E33&amp;" Existing"</f>
+        <v>District heating (SRV) Existing</v>
       </c>
       <c r="M14" s="63" t="s">
         <v>46</v>
@@ -40471,16 +40471,16 @@
         <v>24</v>
       </c>
       <c r="J15" s="63" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:'Regions'!$AD$3)</f>
-        <v>IE,National,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
+        <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
+        <v>IE,National</v>
       </c>
       <c r="K15" s="63" t="str">
-        <f>"FT-"&amp;Commodities!D33&amp;"_1"</f>
-        <v>FT-SRVHET_1</v>
+        <f>"FT-"&amp;D18</f>
+        <v>FT-SRVWIN</v>
       </c>
       <c r="L15" s="63" t="str">
-        <f>Commodities!E33&amp;" in High Urban Density"</f>
-        <v>District heating (SRV) in High Urban Density</v>
+        <f>"Fuel Tech - "&amp;Legend!A47</f>
+        <v>Fuel Tech - Wind</v>
       </c>
       <c r="M15" s="63" t="s">
         <v>46</v>
@@ -40488,9 +40488,7 @@
       <c r="N15" s="63" t="s">
         <v>591</v>
       </c>
-      <c r="O15" s="63" t="s">
-        <v>88</v>
-      </c>
+      <c r="O15" s="63"/>
       <c r="P15" s="63"/>
     </row>
     <row r="16" spans="2:17">
@@ -40507,16 +40505,16 @@
         <v>24</v>
       </c>
       <c r="J16" s="63" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:'Regions'!$AD$3)</f>
-        <v>IE,National,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
+        <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
+        <v>IE,National</v>
       </c>
       <c r="K16" s="63" t="str">
-        <f>"FT-"&amp;Commodities!D33&amp;"_2"</f>
-        <v>FT-SRVHET_2</v>
+        <f>"FT-"&amp;D19</f>
+        <v>FT-SRVH2G</v>
       </c>
       <c r="L16" s="63" t="str">
-        <f>Commodities!E33&amp;" in Medium Urban Density"</f>
-        <v>District heating (SRV) in Medium Urban Density</v>
+        <f>"Fuel Tech - "&amp;Legend!A48</f>
+        <v>Fuel Tech - Hydrogen (gaseous)</v>
       </c>
       <c r="M16" s="63" t="s">
         <v>46</v>
@@ -40524,15 +40522,13 @@
       <c r="N16" s="63" t="s">
         <v>591</v>
       </c>
-      <c r="O16" s="63" t="s">
-        <v>88</v>
-      </c>
+      <c r="O16" s="63"/>
       <c r="P16" s="63"/>
     </row>
     <row r="17" spans="2:17">
       <c r="B17" s="729" t="str">
-        <f t="shared" ref="B17:B20" si="4">K14</f>
-        <v>FT-SRVHET_C</v>
+        <f t="shared" ref="B17" si="4">K14</f>
+        <v>FT-SRVHET_X</v>
       </c>
       <c r="C17" s="728" t="s">
         <v>615</v>
@@ -40549,16 +40545,16 @@
         <v>24</v>
       </c>
       <c r="J17" s="63" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,Regions!$C$3:'Regions'!$AD$3)</f>
-        <v>IE,National,IE-CW,IE-D,IE-KE,IE-KK,IE-LS,IE-LD,IE-LH,IE-MH,IE-OY,IE-WH,IE-WX,IE-WW,IE-CE,IE-CO,IE-KY,IE-LK,IE-TA,IE-WD,IE-G,IE-LM,IE-MO,IE-RN,IE-SO,IE-CN,IE-DL,IE-MN</v>
+        <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
+        <v>IE,National</v>
       </c>
       <c r="K17" s="63" t="str">
-        <f>"FT-"&amp;Commodities!D33&amp;"_3"</f>
-        <v>FT-SRVHET_3</v>
+        <f>"FT-"&amp;D20</f>
+        <v>FT-SRVH2L</v>
       </c>
       <c r="L17" s="63" t="str">
-        <f>Commodities!E33&amp;" in Low Urban Density"</f>
-        <v>District heating (SRV) in Low Urban Density</v>
+        <f>"Fuel Tech - "&amp;Legend!A49</f>
+        <v>Fuel Tech - Hydrogen (liquid)</v>
       </c>
       <c r="M17" s="63" t="s">
         <v>46</v>
@@ -40566,27 +40562,24 @@
       <c r="N17" s="63" t="s">
         <v>591</v>
       </c>
-      <c r="O17" s="63" t="s">
-        <v>88</v>
-      </c>
+      <c r="O17" s="63"/>
       <c r="P17" s="63"/>
     </row>
     <row r="18" spans="2:17">
-      <c r="B18" s="729" t="str">
-        <f t="shared" si="4"/>
-        <v>FT-SRVHET_1</v>
-      </c>
-      <c r="C18" s="728" t="s">
-        <v>615</v>
-      </c>
-      <c r="D18" s="663" t="s">
-        <v>616</v>
-      </c>
-      <c r="E18" s="663">
+      <c r="B18" s="30" t="str">
+        <f>K15</f>
+        <v>FT-SRVWIN</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>563</v>
+      </c>
+      <c r="D18" s="30" t="str">
+        <f>Legend!C47</f>
+        <v>SRVWIN</v>
+      </c>
+      <c r="E18" s="30">
         <v>1</v>
       </c>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
       <c r="I18" s="63" t="s">
         <v>24</v>
       </c>
@@ -40596,11 +40589,11 @@
       </c>
       <c r="K18" s="63" t="str">
         <f>"FT-"&amp;D21</f>
-        <v>FT-SRVWIN</v>
+        <v>FT-SRVBDL</v>
       </c>
       <c r="L18" s="63" t="str">
-        <f>"Fuel Tech - "&amp;Legend!A47</f>
-        <v>Fuel Tech - Wind</v>
+        <f>"Fuel Tech - "&amp;Legend!A50</f>
+        <v>Fuel Tech - Biodiesel</v>
       </c>
       <c r="M18" s="63" t="s">
         <v>46</v>
@@ -40612,213 +40605,94 @@
       <c r="P18" s="63"/>
     </row>
     <row r="19" spans="2:17">
-      <c r="B19" s="729" t="str">
-        <f t="shared" si="4"/>
-        <v>FT-SRVHET_2</v>
-      </c>
-      <c r="C19" s="728" t="s">
-        <v>615</v>
-      </c>
-      <c r="D19" s="663" t="s">
-        <v>616</v>
-      </c>
-      <c r="E19" s="663">
+      <c r="B19" s="30" t="str">
+        <f>K16</f>
+        <v>FT-SRVH2G</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>564</v>
+      </c>
+      <c r="D19" s="30" t="str">
+        <f>Legend!C48</f>
+        <v>SRVH2G</v>
+      </c>
+      <c r="E19" s="30">
         <v>1</v>
       </c>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="I19" s="63" t="s">
+      <c r="I19" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="J19" s="63" t="str">
+      <c r="J19" s="65" t="str">
         <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
         <v>IE,National</v>
       </c>
-      <c r="K19" s="63" t="str">
+      <c r="K19" s="65" t="str">
         <f>"FT-"&amp;D22</f>
-        <v>FT-SRVH2G</v>
-      </c>
-      <c r="L19" s="63" t="str">
-        <f>"Fuel Tech - "&amp;Legend!A48</f>
-        <v>Fuel Tech - Hydrogen (gaseous)</v>
-      </c>
-      <c r="M19" s="63" t="s">
+        <v>FT-SRVETH</v>
+      </c>
+      <c r="L19" s="65" t="str">
+        <f>"Fuel Tech - "&amp;Legend!A51</f>
+        <v>Fuel Tech - Ethanol</v>
+      </c>
+      <c r="M19" s="65" t="s">
         <v>46</v>
       </c>
-      <c r="N19" s="63" t="s">
+      <c r="N19" s="65" t="s">
         <v>591</v>
       </c>
-      <c r="O19" s="63"/>
-      <c r="P19" s="63"/>
+      <c r="O19" s="65"/>
+      <c r="P19" s="65"/>
+      <c r="Q19" s="31"/>
     </row>
     <row r="20" spans="2:17">
-      <c r="B20" s="729" t="str">
-        <f t="shared" si="4"/>
-        <v>FT-SRVHET_3</v>
-      </c>
-      <c r="C20" s="728" t="s">
-        <v>615</v>
-      </c>
-      <c r="D20" s="663" t="s">
-        <v>616</v>
-      </c>
-      <c r="E20" s="663">
+      <c r="B20" s="30" t="str">
+        <f>K17</f>
+        <v>FT-SRVH2L</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>569</v>
+      </c>
+      <c r="D20" s="30" t="str">
+        <f>Legend!C49</f>
+        <v>SRVH2L</v>
+      </c>
+      <c r="E20" s="30">
         <v>1</v>
       </c>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="I20" s="63" t="s">
-        <v>24</v>
-      </c>
-      <c r="J20" s="63" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
-        <v>IE,National</v>
-      </c>
-      <c r="K20" s="63" t="str">
-        <f>"FT-"&amp;D23</f>
-        <v>FT-SRVH2L</v>
-      </c>
-      <c r="L20" s="63" t="str">
-        <f>"Fuel Tech - "&amp;Legend!A49</f>
-        <v>Fuel Tech - Hydrogen (liquid)</v>
-      </c>
-      <c r="M20" s="63" t="s">
-        <v>46</v>
-      </c>
-      <c r="N20" s="63" t="s">
-        <v>591</v>
-      </c>
-      <c r="O20" s="63"/>
-      <c r="P20" s="63"/>
     </row>
     <row r="21" spans="2:17">
       <c r="B21" s="30" t="str">
         <f>K18</f>
-        <v>FT-SRVWIN</v>
+        <v>FT-SRVBDL</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="D21" s="30" t="str">
-        <f>Legend!C47</f>
-        <v>SRVWIN</v>
+        <f>Legend!C50</f>
+        <v>SRVBDL</v>
       </c>
       <c r="E21" s="30">
         <v>1</v>
       </c>
-      <c r="I21" s="63" t="s">
-        <v>24</v>
-      </c>
-      <c r="J21" s="63" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
-        <v>IE,National</v>
-      </c>
-      <c r="K21" s="63" t="str">
-        <f>"FT-"&amp;D24</f>
-        <v>FT-SRVBDL</v>
-      </c>
-      <c r="L21" s="63" t="str">
-        <f>"Fuel Tech - "&amp;Legend!A50</f>
-        <v>Fuel Tech - Biodiesel</v>
-      </c>
-      <c r="M21" s="63" t="s">
-        <v>46</v>
-      </c>
-      <c r="N21" s="63" t="s">
-        <v>591</v>
-      </c>
-      <c r="O21" s="63"/>
-      <c r="P21" s="63"/>
     </row>
     <row r="22" spans="2:17">
-      <c r="B22" s="30" t="str">
+      <c r="B22" s="31" t="str">
         <f>K19</f>
-        <v>FT-SRVH2G</v>
-      </c>
-      <c r="C22" s="30" t="s">
-        <v>564</v>
-      </c>
-      <c r="D22" s="30" t="str">
-        <f>Legend!C48</f>
-        <v>SRVH2G</v>
-      </c>
-      <c r="E22" s="30">
-        <v>1</v>
-      </c>
-      <c r="I22" s="65" t="s">
-        <v>24</v>
-      </c>
-      <c r="J22" s="65" t="str">
-        <f>_xlfn.TEXTJOIN(",",TRUE,IF(LEFT(Regions!$C$3,1)&lt;&gt;"*",Regions!$C$3,""),IF(LEFT(Regions!$D$3,1)&lt;&gt;"*",Regions!$D$3,""))</f>
-        <v>IE,National</v>
-      </c>
-      <c r="K22" s="65" t="str">
-        <f>"FT-"&amp;D25</f>
         <v>FT-SRVETH</v>
       </c>
-      <c r="L22" s="65" t="str">
-        <f>"Fuel Tech - "&amp;Legend!A51</f>
-        <v>Fuel Tech - Ethanol</v>
-      </c>
-      <c r="M22" s="65" t="s">
-        <v>46</v>
-      </c>
-      <c r="N22" s="65" t="s">
-        <v>591</v>
-      </c>
-      <c r="O22" s="65"/>
-      <c r="P22" s="65"/>
-      <c r="Q22" s="31"/>
-    </row>
-    <row r="23" spans="2:17">
-      <c r="B23" s="30" t="str">
-        <f>K20</f>
-        <v>FT-SRVH2L</v>
-      </c>
-      <c r="C23" s="30" t="s">
-        <v>569</v>
-      </c>
-      <c r="D23" s="30" t="str">
-        <f>Legend!C49</f>
-        <v>SRVH2L</v>
-      </c>
-      <c r="E23" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="2:17">
-      <c r="B24" s="30" t="str">
-        <f>K21</f>
-        <v>FT-SRVBDL</v>
-      </c>
-      <c r="C24" s="30" t="s">
-        <v>560</v>
-      </c>
-      <c r="D24" s="30" t="str">
-        <f>Legend!C50</f>
-        <v>SRVBDL</v>
-      </c>
-      <c r="E24" s="30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="2:17">
-      <c r="B25" s="31" t="str">
-        <f>K22</f>
-        <v>FT-SRVETH</v>
-      </c>
-      <c r="C25" s="31" t="s">
+      <c r="C22" s="31" t="s">
         <v>559</v>
       </c>
-      <c r="D25" s="31" t="str">
+      <c r="D22" s="31" t="str">
         <f>Legend!C51</f>
         <v>SRVETH</v>
       </c>
-      <c r="E25" s="31">
+      <c r="E22" s="31">
         <v>1</v>
       </c>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>